<commit_message>
Retirando uma coluna da tabela
</commit_message>
<xml_diff>
--- a/relatorio_casas_de_aposta.xlsx
+++ b/relatorio_casas_de_aposta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,11 +469,6 @@
           <t>Nota do Consumidor</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Nota Geral</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -511,11 +506,6 @@
           <t>9.85</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -553,11 +543,6 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -595,11 +580,6 @@
           <t>9.55</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -637,11 +617,6 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -679,11 +654,6 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -719,11 +689,6 @@
       <c r="G7" t="inlineStr">
         <is>
           <t>--</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalizando Desafio com comentários e guias no código
</commit_message>
<xml_diff>
--- a/relatorio_casas_de_aposta.xlsx
+++ b/relatorio_casas_de_aposta.xlsx
@@ -525,22 +525,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>98.9%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>98.4%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>99.8%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>9.5</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>98.1%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">

</xml_diff>